<commit_message>
Added files via upload
</commit_message>
<xml_diff>
--- a/Tool Comparison.xlsx
+++ b/Tool Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10632"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19236" windowHeight="9168"/>
   </bookViews>
   <sheets>
     <sheet name="Triage Tool Comparison" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="121">
   <si>
     <t>TR3Secure</t>
   </si>
@@ -386,18 +386,7 @@
     <t>IRTriage 2</t>
   </si>
   <si>
-    <t>route print</t>
-  </si>
-  <si>
-    <t>ipconfig /displaydns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c:\windows\system32\drivers\etc\hosts
-c:\windows\system32\drivers\etc\hosts
-</t>
-  </si>
-  <si>
-    <t>Sysinternals\tcpvcon -anc</t>
+    <t>tools\RawCopy.exe %WINDIR%\AppCompat\Programs\RecentFileCache.bcf %c_drive%:\Data-%case%\%computername%-%timestamp%\preserved-files\AppCompat</t>
   </si>
 </sst>
 </file>
@@ -681,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -731,10 +720,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -907,6 +892,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -942,6 +944,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1094,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
@@ -1168,13 +1187,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="22"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>120</v>
+      <c r="C4" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
@@ -1189,8 +1208,8 @@
       <c r="B5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>121</v>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14" t="s">
@@ -1231,8 +1250,8 @@
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>122</v>
+      <c r="C8" s="14" t="s">
+        <v>5</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1280,7 +1299,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14" t="s">
@@ -1323,7 +1342,9 @@
       <c r="B14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="14"/>
+      <c r="C14" s="14" t="s">
+        <v>5</v>
+      </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="15" t="s">
@@ -1366,7 +1387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
@@ -1378,7 +1399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="2" t="s">
         <v>73</v>
@@ -1390,7 +1411,7 @@
       </c>
       <c r="F18" s="15"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
       <c r="B19" s="2" t="s">
         <v>74</v>
@@ -1402,7 +1423,7 @@
       </c>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="2" t="s">
         <v>16</v>
@@ -1414,7 +1435,7 @@
       </c>
       <c r="F20" s="15"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="2" t="s">
         <v>17</v>
@@ -1426,7 +1447,7 @@
       </c>
       <c r="F21" s="15"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="2" t="s">
         <v>18</v>
@@ -1438,7 +1459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="2" t="s">
         <v>19</v>
@@ -1450,7 +1471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="2" t="s">
         <v>81</v>
@@ -1462,7 +1483,7 @@
       </c>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="2" t="s">
         <v>82</v>
@@ -1480,7 +1501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="2" t="s">
         <v>83</v>
@@ -1493,8 +1514,11 @@
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="22"/>
       <c r="B27" s="2" t="s">
         <v>84</v>
@@ -1506,7 +1530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="22"/>
       <c r="B28" s="2" t="s">
         <v>85</v>
@@ -1520,7 +1544,7 @@
       <c r="E28" s="14"/>
       <c r="F28" s="15"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
       <c r="B29" s="2" t="s">
         <v>86</v>
@@ -1534,7 +1558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="22"/>
       <c r="B30" s="2" t="s">
         <v>20</v>
@@ -1550,7 +1574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="22"/>
       <c r="B31" s="2" t="s">
         <v>21</v>
@@ -1566,7 +1590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="22"/>
       <c r="B32" s="2" t="s">
         <v>22</v>
@@ -2661,7 +2685,7 @@
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A59:A110"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:F3 C6:F52 D4:F5">
+  <conditionalFormatting sqref="C3:F52">
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",C3)))</formula>
     </cfRule>

</xml_diff>